<commit_message>
POC for 1000 users, Databse connectivity, Exteracting data from the database.
</commit_message>
<xml_diff>
--- a/datafiles/kiteDDT.xlsx
+++ b/datafiles/kiteDDT.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11011"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gourav.sharma\IdeaProjects\falcon_project\datafiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/Desktop/untitled folder/falcon_project/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C41A1D01-9566-B94F-82B4-5B22568AF887}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="12340" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
@@ -17,18 +18,16 @@
     <sheet name="CreateAdmin" sheetId="3" r:id="rId3"/>
     <sheet name="CreateNewTransfer" sheetId="4" r:id="rId4"/>
     <sheet name="ViewTransfer" sheetId="5" r:id="rId5"/>
+    <sheet name="DartLogin" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="69">
   <si>
     <t>UserName</t>
   </si>
@@ -158,9 +157,6 @@
     <t>Super Admin</t>
   </si>
   <si>
-    <t>Readonly Admin</t>
-  </si>
-  <si>
     <t>FinancialProduct</t>
   </si>
   <si>
@@ -218,48 +214,42 @@
     <t>Haryana</t>
   </si>
   <si>
-    <t>Clifford</t>
-  </si>
-  <si>
-    <t>Gislason</t>
-  </si>
-  <si>
-    <t>htPY2@mailinator.com</t>
-  </si>
-  <si>
-    <t>9826035585</t>
-  </si>
-  <si>
-    <t>Louie</t>
-  </si>
-  <si>
-    <t>Bechtelar</t>
-  </si>
-  <si>
-    <t>ek8A9@mailinator.com</t>
-  </si>
-  <si>
-    <t>982608000</t>
-  </si>
-  <si>
-    <t>Austin</t>
-  </si>
-  <si>
-    <t>Hudson</t>
-  </si>
-  <si>
-    <t>BRgkE@mailinator.com</t>
-  </si>
-  <si>
-    <t>9826012755</t>
+    <t>9826092386</t>
+  </si>
+  <si>
+    <t>8BB@mailinator.com</t>
+  </si>
+  <si>
+    <t>Gourav</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>9826030697</t>
+  </si>
+  <si>
+    <t>9826071406</t>
+  </si>
+  <si>
+    <t>9826034718</t>
+  </si>
+  <si>
+    <t>9826035759</t>
+  </si>
+  <si>
+    <t>9826066553</t>
+  </si>
+  <si>
+    <t>9826038277</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,6 +287,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -344,7 +341,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -364,6 +361,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -678,17 +678,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.6640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -705,36 +705,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U3" sqref="U3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="5" max="6" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="5" max="6" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.5" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="12.1640625" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="28.7109375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="23.42578125" collapsed="true"/>
-    <col min="26" max="26" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="13.33203125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="11.33203125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="12.33203125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="17.6640625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="20.33203125" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="13.5" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="26.33203125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="23.5" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="27.33203125" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="20.5" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="28.6640625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="23.5" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="9.5" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:31" s="6" customFormat="1">
@@ -835,15 +835,15 @@
     <row r="2" spans="1:31">
       <c r="A2" t="str">
         <f ca="1">CONCATENATE(B2,"11")</f>
-        <v>vszpl11</v>
+        <v>lrgjb11</v>
       </c>
       <c r="B2" t="str">
         <f ca="1">LOWER(CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90)) &amp; CHAR(RANDBETWEEN(65,90))&amp; CHAR(RANDBETWEEN(65,90)))</f>
-        <v>vszpl</v>
+        <v>lrgjb</v>
       </c>
       <c r="C2" t="str">
         <f ca="1">B2</f>
-        <v>vszpl</v>
+        <v>lrgjb</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -871,7 +871,7 @@
       </c>
       <c r="L2" s="7" t="str">
         <f ca="1">CONCATENATE(A2,"@mailinator.com")</f>
-        <v>vszpl11@mailinator.com</v>
+        <v>lrgjb11@mailinator.com</v>
       </c>
       <c r="M2" t="s">
         <v>33</v>
@@ -899,7 +899,7 @@
       </c>
       <c r="U2" t="str">
         <f ca="1">UPPER(CONCATENATE(B2,"9009G"))</f>
-        <v>VSZPL9009G</v>
+        <v>LRGJB9009G</v>
       </c>
       <c r="V2" t="s">
         <v>33</v>
@@ -909,15 +909,15 @@
       </c>
       <c r="X2" t="str">
         <f ca="1">CONCATENATE(900,RANDBETWEEN(1000000,9999999))</f>
-        <v>9005245727</v>
+        <v>9006596351</v>
       </c>
       <c r="Y2" t="str">
         <f ca="1">CONCATENATE(900,RANDBETWEEN(1000000,9999999))</f>
-        <v>9007634558</v>
+        <v>9007336701</v>
       </c>
       <c r="Z2" t="str">
         <f ca="1">L2</f>
-        <v>vszpl11@mailinator.com</v>
+        <v>lrgjb11@mailinator.com</v>
       </c>
       <c r="AA2" t="s">
         <v>33</v>
@@ -926,10 +926,10 @@
         <v>33</v>
       </c>
       <c r="AC2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD2" t="s">
         <v>58</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>59</v>
       </c>
       <c r="AE2" s="8">
         <v>133001</v>
@@ -942,21 +942,21 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="15.7109375" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="15.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="10.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.33203125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.83203125" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
@@ -986,7 +986,7 @@
     <row r="2" spans="1:7">
       <c r="A2" t="str">
         <f ca="1">AddEnterprise!B2</f>
-        <v>vszpl</v>
+        <v>lrgjb</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -995,53 +995,48 @@
         <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F2" t="s">
-        <v>70</v>
+        <v>62</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>60</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="C3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="21.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="16.5703125" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="22.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.5" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="21.83203125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.6640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="16.5" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="22.1640625" collapsed="true"/>
     <col min="7" max="7" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.1640625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="27.5" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75">
+    <row r="1" spans="1:9" ht="17">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1049,31 +1044,31 @@
         <v>5</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="5" t="s">
+      <c r="H1" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="I1" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="I1" s="5" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="str">
         <f ca="1">AddEnterprise!B2</f>
-        <v>vszpl</v>
+        <v>lrgjb</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
@@ -1107,55 +1102,100 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="9.5703125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="23.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="33.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="1" width="21.0" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="15.5" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="9.5" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="23.6640625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="33.5" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="15.6640625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" style="1" width="21.0" collapsed="true"/>
+    <col min="7" max="16384" style="1" width="9.1640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="2" t="s">
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="str">
+        <f ca="1">AddEnterprise!B2</f>
+        <v>lrgjb</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>57</v>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.83203125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="str">
+        <f ca="1">CONCATENATE(AddEnterprise!B2,"11")</f>
+        <v>lrgjb11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>